<commit_message>
Individual Scenario KDMA scores (UK DATA) (#396)
* update headers

* var defs
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/AggregateResults/Variable Definitions/UK_Variables.xlsx
+++ b/dashboard-ui/src/components/AggregateResults/Variable Definitions/UK_Variables.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>Variable</t>
   </si>
@@ -64,12 +64,24 @@
     <t>MJ_KDMA_Text</t>
   </si>
   <si>
+    <t>MJ_KDMA_Text_Narr</t>
+  </si>
+  <si>
+    <t>MJ_KDMA_Text_NonNarr</t>
+  </si>
+  <si>
     <t>MJ_KDMA_Sim</t>
   </si>
   <si>
     <t>IO_KDMA_Text</t>
   </si>
   <si>
+    <t>IO_KDMA_Text_Narr</t>
+  </si>
+  <si>
+    <t>IO_KDMA_Text_NonNarr</t>
+  </si>
+  <si>
     <t>IO_KDMA_Sim</t>
   </si>
   <si>
@@ -136,12 +148,24 @@
     <t>Moral Judgement KDMA measurement for all Adept text scenarios combined</t>
   </si>
   <si>
+    <t>Moral Judgement KDMA measurement from narrative Adept text scenario only (MJ5)</t>
+  </si>
+  <si>
+    <t>Moral Judgement KDMA measurement from non narrative Adept text scenario only (MJ1)</t>
+  </si>
+  <si>
     <t>Moral Judgement KDMA measurement for the Adept Sim scenario</t>
   </si>
   <si>
     <t>Ingroup Bias KDMA measurement for all Adept text scenarios combined</t>
   </si>
   <si>
+    <t>Ingroup Bias KDMA measurement from narrative Adept text scenario only (MJ5)</t>
+  </si>
+  <si>
+    <t>Ingroup Bias KDMA measurement from non narrative Adept text scenario only (IO1)</t>
+  </si>
+  <si>
     <t>Ingroup Bias KDMA measurement for the Adept Sim scenario</t>
   </si>
   <si>
@@ -176,9 +200,6 @@
   </si>
   <si>
     <t>Calculation</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Average the numerical responses to 3 items using: -2 = strongly disagree, -1= disagree, 0 = neutral, 1 = agree, 2 = strongly agree</t>
@@ -245,12 +266,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -558,31 +576,35 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="100.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="3" width="67.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="3" width="61.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="3" width="40.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="3" width="109.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="3" width="60.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="3" width="65.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="3" width="71.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="3" width="68.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="3" width="58.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="3" width="63.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="100.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="67.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="61.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="40.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="109.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="2" width="60.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="2" width="65.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="2" width="71.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="2" width="68.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="2" width="87.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="2" width="78.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="2" width="58.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="2" width="63.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="2" width="82.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="2" width="73.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -643,300 +665,366 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>